<commit_message>
how much costs 1000 kkal
</commit_message>
<xml_diff>
--- a/graphs.xlsx
+++ b/graphs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="18195" windowHeight="12075"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -58,11 +58,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,7 +95,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -131,11 +131,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -173,6 +201,26 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -189,24 +237,12 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -226,15 +262,13 @@
           </c:marker>
           <c:trendline>
             <c:trendlineType val="exp"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$A$2:$A$29</c:f>
+              <c:f>Лист1!$A$2:$A$35</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:formatCode>dd/mm/yyyy</c:formatCode>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>43556</c:v>
                 </c:pt>
@@ -318,16 +352,34 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>43583</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43584</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43585</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43586</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43587</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43588</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43589</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$F$2:$F$29</c:f>
+              <c:f>Лист1!$F$2:$F$35</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>13.218645246979952</c:v>
                 </c:pt>
@@ -411,11 +463,28 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>17.236662106703147</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>15.520762423417292</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14.046822742474916</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>20.089439284485724</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>21.151832460732983</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>16.064257028112451</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>12.94176207068193</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -436,15 +505,13 @@
           </c:marker>
           <c:trendline>
             <c:trendlineType val="exp"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$A$2:$A$29</c:f>
+              <c:f>Лист1!$A$2:$A$35</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:formatCode>dd/mm/yyyy</c:formatCode>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>43556</c:v>
                 </c:pt>
@@ -528,16 +595,34 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>43583</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43584</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43585</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43586</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43587</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43588</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43589</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$G$2:$G$29</c:f>
+              <c:f>Лист1!$G$2:$G$35</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>34.551894250838025</c:v>
                 </c:pt>
@@ -621,11 +706,28 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>27.086183310533517</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28.795098706603135</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>25.88628762541806</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>26.934984520123841</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>23.560209424083769</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>23.329682365826944</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>21.951219512195124</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -646,15 +748,13 @@
           </c:marker>
           <c:trendline>
             <c:trendlineType val="exp"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$A$2:$A$29</c:f>
+              <c:f>Лист1!$A$2:$A$35</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:formatCode>dd/mm/yyyy</c:formatCode>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>43556</c:v>
                 </c:pt>
@@ -738,16 +838,34 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>43583</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43584</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43585</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43586</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43587</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43588</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43589</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$H$2:$H$29</c:f>
+              <c:f>Лист1!$H$2:$H$35</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>52.229460502182022</c:v>
                 </c:pt>
@@ -831,56 +949,60 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>55.677154582763336</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>55.684138869979584</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>60.066889632107021</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>52.975576195390438</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>55.287958115183244</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>60.606060606060609</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>65.107018417122944</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="75872512"/>
-        <c:axId val="75882496"/>
+        <c:axId val="61068032"/>
+        <c:axId val="61069568"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="75872512"/>
+        <c:axId val="61068032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:numFmt formatCode="dd/mm/yyyy" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75882496"/>
+        <c:crossAx val="61069568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="75882496"/>
+        <c:axId val="61069568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:minorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75872512"/>
+        <c:crossAx val="61068032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -889,11 +1011,10 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -901,24 +1022,12 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:areaChart>
         <c:grouping val="percentStacked"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="5"/>
           <c:order val="0"/>
@@ -935,10 +1044,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$A$2:$A$29</c:f>
+              <c:f>Лист1!$A$2:$A$35</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:formatCode>dd/mm/yyyy</c:formatCode>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>43556</c:v>
                 </c:pt>
@@ -1022,16 +1131,34 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>43583</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43584</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43585</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43586</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43587</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43588</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43589</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$F$2:$F$30</c:f>
+              <c:f>Лист1!$F$2:$F$57</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="56"/>
                 <c:pt idx="0">
                   <c:v>13.218645246979952</c:v>
                 </c:pt>
@@ -1117,7 +1244,88 @@
                   <c:v>17.236662106703147</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>15.370691276494002</c:v>
+                  <c:v>15.520762423417292</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14.046822742474916</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>20.089439284485724</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>21.151832460732983</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>16.064257028112451</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>12.94176207068193</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>16.78119349005425</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>13.818860877684408</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>10.87866108786611</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>12.598425196850393</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>15.151515151515152</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>16.029143897996356</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>16.883116883116884</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>14.142165984369184</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>14.057507987220447</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>15.56420233463035</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>12.348993288590604</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>13.959917069799586</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>16.059067835717585</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>18.135283363802561</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>10.542635658914728</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>14.809782608695651</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>17.318255250403876</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>17.185554171855539</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>13.636363636363635</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>13.819825637713917</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>18.946350894151763</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>15.179823979728445</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1139,10 +1347,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$A$2:$A$29</c:f>
+              <c:f>Лист1!$A$2:$A$35</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:formatCode>dd/mm/yyyy</c:formatCode>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>43556</c:v>
                 </c:pt>
@@ -1226,16 +1434,34 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>43583</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43584</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43585</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43586</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43587</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43588</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43589</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$G$2:$G$30</c:f>
+              <c:f>Лист1!$G$2:$G$57</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="56"/>
                 <c:pt idx="0">
                   <c:v>34.551894250838025</c:v>
                 </c:pt>
@@ -1321,7 +1547,88 @@
                   <c:v>27.086183310533517</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>27.712801750748852</c:v>
+                  <c:v>28.795098706603135</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>25.88628762541806</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>26.934984520123841</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>23.560209424083769</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>23.329682365826944</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>21.951219512195124</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>26.365280289330922</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>59.663865546218489</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>42.928870292887026</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>51.098217985909656</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>46.022727272727273</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>22.950819672131146</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>33.116883116883116</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>34.499441756605883</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>34.094020994979459</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>21.819814426818319</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>25.369127516778523</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>29.232895646164479</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>26.165205353022614</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>28.628884826325411</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>36.744186046511629</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>26.902173913043477</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>26.462035541195476</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>23.536737235367372</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>26.74825174825175</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>27.026154342912495</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>23.054615756404058</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>27.210593511955178</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1343,10 +1650,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$A$2:$A$29</c:f>
+              <c:f>Лист1!$A$2:$A$35</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:formatCode>dd/mm/yyyy</c:formatCode>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>43556</c:v>
                 </c:pt>
@@ -1430,16 +1737,34 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>43583</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43584</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43585</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43586</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43587</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43588</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43589</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$H$2:$H$30</c:f>
+              <c:f>Лист1!$H$2:$H$57</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="56"/>
                 <c:pt idx="0">
                   <c:v>52.229460502182022</c:v>
                 </c:pt>
@@ -1525,53 +1850,120 @@
                   <c:v>55.677154582763336</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>56.916506972757148</c:v>
+                  <c:v>55.684138869979584</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>60.066889632107021</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>52.975576195390438</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>55.287958115183244</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>60.606060606060609</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>65.107018417122944</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>56.853526220614825</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>26.517273576097107</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>46.19246861924686</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>36.303356817239951</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38.825757575757578</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>61.020036429872491</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>51.358392259024932</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>51.848471017800094</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>62.61598323855133</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>62.281879194630875</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>56.807187284035933</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>57.775726811259808</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>53.235831809872025</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>52.713178294573652</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>58.288043478260867</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>56.219709208400644</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>59.277708592777088</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>59.615384615384613</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>59.15402001937359</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>57.999033349444176</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>57.609582508316386</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="77218944"/>
-        <c:axId val="77220480"/>
+        <c:axId val="61487744"/>
+        <c:axId val="61497728"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="77218944"/>
+        <c:axId val="61487744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:numFmt formatCode="dd/mm/yyyy" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77220480"/>
+        <c:crossAx val="61497728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="77220480"/>
+        <c:axId val="61497728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77218944"/>
+        <c:crossAx val="61487744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1579,15 +1971,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1595,24 +1985,22 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.4376497774734679E-2"/>
+          <c:y val="2.2696490158909403E-2"/>
+          <c:w val="0.87402787287458628"/>
+          <c:h val="0.74129568136472967"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -1632,10 +2020,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$A$2:$A$29</c:f>
+              <c:f>Лист1!$A$2:$A$49</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:formatCode>dd/mm/yyyy</c:formatCode>
+                <c:ptCount val="48"/>
                 <c:pt idx="0">
                   <c:v>43556</c:v>
                 </c:pt>
@@ -1719,16 +2107,76 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>43583</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43584</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43585</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43586</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43587</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43588</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43589</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>43590</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>43591</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>43592</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>43593</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>43594</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>43595</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>43596</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>43597</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43598</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43599</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>43600</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>43601</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>43602</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>43603</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$E$2:$E$29</c:f>
+              <c:f>Лист1!$E$2:$E$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="48"/>
                 <c:pt idx="0" formatCode="0">
                   <c:v>3162.2</c:v>
                 </c:pt>
@@ -1812,28 +2260,77 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>2924</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2938</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2990</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2907</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1910</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2739</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2765</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2142</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2390</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2413</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2112</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2196</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1848</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2687</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2191</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3341</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2235</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2894</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2167</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2735</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="77255040"/>
-        <c:axId val="77256576"/>
+        <c:axId val="61533184"/>
+        <c:axId val="61543168"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="1"/>
@@ -1853,10 +2350,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$A$2:$A$29</c:f>
+              <c:f>Лист1!$A$2:$A$49</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:formatCode>dd/mm/yyyy</c:formatCode>
+                <c:ptCount val="48"/>
                 <c:pt idx="0">
                   <c:v>43556</c:v>
                 </c:pt>
@@ -1940,16 +2437,76 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>43583</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43584</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43585</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43586</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43587</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43588</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43589</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>43590</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>43591</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>43592</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>43593</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>43594</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>43595</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>43596</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>43597</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43598</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43599</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>43600</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>43601</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>43602</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>43603</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$I$2:$I$29</c:f>
+              <c:f>Лист1!$I$2:$I$49</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="48"/>
                 <c:pt idx="0">
                   <c:v>59.1</c:v>
                 </c:pt>
@@ -2033,85 +2590,124 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>60.4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>60.4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>60.4</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>60.4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>60.4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>60.4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>60.4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>60.4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>60.4</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>60.4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>60.4</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>60.4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>60.4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>60.4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>60.4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>60.4</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>60.4</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>60.4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>60.4</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>60.4</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>61.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="89658496"/>
-        <c:axId val="77258112"/>
+        <c:axId val="61558784"/>
+        <c:axId val="61544704"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="77255040"/>
+        <c:axId val="61533184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:numFmt formatCode="dd/mm/yyyy" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77256576"/>
+        <c:crossAx val="61543168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="77256576"/>
+        <c:axId val="61543168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77255040"/>
+        <c:crossAx val="61533184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77258112"/>
+        <c:axId val="61544704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="r"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89658496"/>
+        <c:crossAx val="61558784"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:dateAx>
-        <c:axId val="89658496"/>
+        <c:axId val="61558784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77258112"/>
+        <c:numFmt formatCode="dd/mm/yyyy" sourceLinked="1"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="61544704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -2120,11 +2716,10 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2132,29 +2727,16 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2169,13 +2751,12 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$A$2:$A$29</c:f>
+              <c:f>Лист1!$A$2:$A$35</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:formatCode>dd/mm/yyyy</c:formatCode>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>43556</c:v>
                 </c:pt>
@@ -2259,6 +2840,24 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>43583</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43584</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43585</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43586</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43587</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43588</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43589</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2357,59 +2956,42 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="89670016"/>
-        <c:axId val="89671552"/>
+        <c:axId val="61577856"/>
+        <c:axId val="61579648"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="89670016"/>
+        <c:axId val="61577856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:numFmt formatCode="dd/mm/yyyy" sourceLinked="1"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="89671552"/>
+        <c:crossAx val="61579648"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="89671552"/>
+        <c:axId val="61579648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89670016"/>
+        <c:crossAx val="61577856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2420,15 +3002,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>161924</xdr:colOff>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>4760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2449,16 +3031,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>295274</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>352424</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2479,16 +3061,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>147636</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>71436</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2509,16 +3091,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>80961</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>109536</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2615,7 +3197,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2650,7 +3231,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -2826,19 +3406,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2879,7 +3459,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" s="4">
         <v>43556</v>
       </c>
@@ -2912,16 +3492,16 @@
         <v>59.1</v>
       </c>
       <c r="J2" s="5">
-        <f>F2-20</f>
-        <v>-6.7813547530200484</v>
+        <f>B2-126</f>
+        <v>-21.5</v>
       </c>
       <c r="K2" s="5">
-        <f>G2-25</f>
-        <v>9.5518942508380249</v>
+        <f>C2-88</f>
+        <v>33.400000000000006</v>
       </c>
       <c r="L2" s="5">
-        <f>H2-55</f>
-        <v>-2.7705394978179783</v>
+        <f>D2-450</f>
+        <v>-37.100000000000023</v>
       </c>
       <c r="M2" s="5">
         <f>E2-3100</f>
@@ -2929,7 +3509,7 @@
       </c>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" s="4">
         <v>43557</v>
       </c>
@@ -2943,43 +3523,43 @@
         <v>227</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E29" si="0">(B3+D3)*4+C3*9</f>
+        <f t="shared" ref="E3:E56" si="0">(B3+D3)*4+C3*9</f>
         <v>2389</v>
       </c>
       <c r="F3" s="5">
-        <f t="shared" ref="F3:F29" si="1">B3*4/$E3*100</f>
+        <f t="shared" ref="F3:F56" si="1">B3*4/$E3*100</f>
         <v>20.929259104227711</v>
       </c>
       <c r="G3" s="5">
-        <f t="shared" ref="G3:G29" si="2">C3*9/$E3*100</f>
+        <f t="shared" ref="G3:G56" si="2">C3*9/$E3*100</f>
         <v>41.063206362494768</v>
       </c>
       <c r="H3" s="5">
-        <f t="shared" ref="H3:H29" si="3">D3*4/$E3*100</f>
+        <f t="shared" ref="H3:H56" si="3">D3*4/$E3*100</f>
         <v>38.007534533277521</v>
       </c>
       <c r="I3" s="13">
         <v>59.1</v>
       </c>
       <c r="J3" s="5">
-        <f t="shared" ref="J3:J29" si="4">F3-20</f>
-        <v>0.92925910422771096</v>
+        <f t="shared" ref="J3:J56" si="4">B3-126</f>
+        <v>-1</v>
       </c>
       <c r="K3" s="5">
-        <f t="shared" ref="K3:K29" si="5">G3-25</f>
-        <v>16.063206362494768</v>
+        <f t="shared" ref="K3:K56" si="5">C3-88</f>
+        <v>21</v>
       </c>
       <c r="L3" s="5">
-        <f t="shared" ref="L3:L29" si="6">H3-55</f>
-        <v>-16.992465466722479</v>
+        <f t="shared" ref="L3:L56" si="6">D3-450</f>
+        <v>-223</v>
       </c>
       <c r="M3" s="5">
-        <f t="shared" ref="M3:M29" si="7">E3-3100</f>
+        <f t="shared" ref="M3:M56" si="7">E3-3100</f>
         <v>-711</v>
       </c>
       <c r="N3" s="6"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" s="4">
         <v>43558</v>
       </c>
@@ -3013,15 +3593,15 @@
       </c>
       <c r="J4" s="5">
         <f t="shared" si="4"/>
-        <v>-9.5229186155285301</v>
+        <v>-70</v>
       </c>
       <c r="K4" s="5">
         <f t="shared" si="5"/>
-        <v>11.202057998129092</v>
+        <v>-2</v>
       </c>
       <c r="L4" s="5">
         <f t="shared" si="6"/>
-        <v>-1.6791393826005674</v>
+        <v>-165</v>
       </c>
       <c r="M4" s="5">
         <f t="shared" si="7"/>
@@ -3029,7 +3609,7 @@
       </c>
       <c r="N4" s="6"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" s="4">
         <v>43559</v>
       </c>
@@ -3063,15 +3643,15 @@
       </c>
       <c r="J5" s="5">
         <f t="shared" si="4"/>
-        <v>-7.9518072289156621</v>
+        <v>-46</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" si="5"/>
-        <v>0.7530120481927689</v>
+        <v>-12</v>
       </c>
       <c r="L5" s="5">
         <f t="shared" si="6"/>
-        <v>7.1987951807228896</v>
+        <v>-37</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" si="7"/>
@@ -3079,7 +3659,7 @@
       </c>
       <c r="N5" s="6"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="A6" s="4">
         <v>43560</v>
       </c>
@@ -3113,15 +3693,15 @@
       </c>
       <c r="J6" s="5">
         <f t="shared" si="4"/>
-        <v>-6.1377108983128146</v>
+        <v>-50</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" si="5"/>
-        <v>-3.2489740082079344</v>
+        <v>-35</v>
       </c>
       <c r="L6" s="5">
         <f t="shared" si="6"/>
-        <v>9.386684906520756</v>
+        <v>-97</v>
       </c>
       <c r="M6" s="5">
         <f t="shared" si="7"/>
@@ -3129,107 +3709,107 @@
       </c>
       <c r="N6" s="6"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A7" s="19">
         <v>43561</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="20">
         <v>99</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="20">
         <v>114</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="20">
         <v>282</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="20">
         <f t="shared" si="0"/>
         <v>2550</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="21">
         <f t="shared" si="1"/>
         <v>15.529411764705884</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="21">
         <f t="shared" si="2"/>
         <v>40.235294117647058</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="21">
         <f t="shared" si="3"/>
         <v>44.235294117647058</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="22">
         <v>59.1</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="21">
         <f t="shared" si="4"/>
-        <v>-4.470588235294116</v>
-      </c>
-      <c r="K7" s="5">
+        <v>-27</v>
+      </c>
+      <c r="K7" s="21">
         <f t="shared" si="5"/>
-        <v>15.235294117647058</v>
-      </c>
-      <c r="L7" s="5">
+        <v>26</v>
+      </c>
+      <c r="L7" s="21">
         <f t="shared" si="6"/>
-        <v>-10.764705882352942</v>
-      </c>
-      <c r="M7" s="5">
+        <v>-168</v>
+      </c>
+      <c r="M7" s="21">
         <f t="shared" si="7"/>
         <v>-550</v>
       </c>
       <c r="N7" s="6"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+    <row r="8" spans="1:14">
+      <c r="A8" s="15">
         <v>43562</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="16">
         <v>67</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="16">
         <v>56</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="16">
         <v>281</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="16">
         <f t="shared" si="0"/>
         <v>1896</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="17">
         <f t="shared" si="1"/>
         <v>14.135021097046414</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="17">
         <f t="shared" si="2"/>
         <v>26.582278481012654</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="17">
         <f t="shared" si="3"/>
         <v>59.282700421940923</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="18">
         <v>58.9</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="17">
         <f t="shared" si="4"/>
-        <v>-5.8649789029535864</v>
-      </c>
-      <c r="K8" s="5">
+        <v>-59</v>
+      </c>
+      <c r="K8" s="17">
         <f t="shared" si="5"/>
-        <v>1.5822784810126542</v>
-      </c>
-      <c r="L8" s="5">
+        <v>-32</v>
+      </c>
+      <c r="L8" s="17">
         <f t="shared" si="6"/>
-        <v>4.2827004219409233</v>
-      </c>
-      <c r="M8" s="5">
+        <v>-169</v>
+      </c>
+      <c r="M8" s="17">
         <f t="shared" si="7"/>
         <v>-1204</v>
       </c>
       <c r="N8" s="6"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9" s="4">
         <v>43563</v>
       </c>
@@ -3263,15 +3843,15 @@
       </c>
       <c r="J9" s="5">
         <f t="shared" si="4"/>
-        <v>-3.6663770634231128</v>
+        <v>-32</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" si="5"/>
-        <v>18.006081668114682</v>
+        <v>22</v>
       </c>
       <c r="L9" s="5">
         <f t="shared" si="6"/>
-        <v>-14.339704604691576</v>
+        <v>-216</v>
       </c>
       <c r="M9" s="5">
         <f t="shared" si="7"/>
@@ -3279,7 +3859,7 @@
       </c>
       <c r="N9" s="6"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10" s="4">
         <v>43564</v>
       </c>
@@ -3313,15 +3893,15 @@
       </c>
       <c r="J10" s="5">
         <f t="shared" si="4"/>
-        <v>-4.3226788432267895</v>
+        <v>-23</v>
       </c>
       <c r="K10" s="5">
         <f t="shared" si="5"/>
-        <v>6.506849315068493</v>
+        <v>4</v>
       </c>
       <c r="L10" s="5">
         <f t="shared" si="6"/>
-        <v>-2.1841704718417034</v>
+        <v>-103</v>
       </c>
       <c r="M10" s="5">
         <f t="shared" si="7"/>
@@ -3329,7 +3909,7 @@
       </c>
       <c r="N10" s="6"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" s="9">
         <v>43565</v>
       </c>
@@ -3363,15 +3943,15 @@
       </c>
       <c r="J11" s="11">
         <f t="shared" si="4"/>
-        <v>-7.1490280777537798</v>
+        <v>-7</v>
       </c>
       <c r="K11" s="11">
         <f t="shared" si="5"/>
-        <v>1.2419006479481638</v>
+        <v>20</v>
       </c>
       <c r="L11" s="11">
         <f t="shared" si="6"/>
-        <v>5.9071274298056196</v>
+        <v>114</v>
       </c>
       <c r="M11" s="11">
         <f t="shared" si="7"/>
@@ -3379,7 +3959,7 @@
       </c>
       <c r="N11" s="6"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12" s="4">
         <v>43566</v>
       </c>
@@ -3413,15 +3993,15 @@
       </c>
       <c r="J12" s="5">
         <f t="shared" si="4"/>
-        <v>-1.8811309867282162</v>
+        <v>31</v>
       </c>
       <c r="K12" s="5">
         <f t="shared" si="5"/>
-        <v>-2.6687824581650297</v>
+        <v>-2</v>
       </c>
       <c r="L12" s="5">
         <f t="shared" si="6"/>
-        <v>4.5499134448932423</v>
+        <v>66</v>
       </c>
       <c r="M12" s="5">
         <f t="shared" si="7"/>
@@ -3429,7 +4009,7 @@
       </c>
       <c r="N12" s="6"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="A13" s="4">
         <v>43567</v>
       </c>
@@ -3463,15 +4043,15 @@
       </c>
       <c r="J13" s="5">
         <f t="shared" si="4"/>
-        <v>-3.7819873712196745</v>
+        <v>-4</v>
       </c>
       <c r="K13" s="5">
         <f t="shared" si="5"/>
-        <v>-3.1655034895314067</v>
+        <v>-15</v>
       </c>
       <c r="L13" s="5">
         <f t="shared" si="6"/>
-        <v>6.9474908607510741</v>
+        <v>16</v>
       </c>
       <c r="M13" s="5">
         <f t="shared" si="7"/>
@@ -3479,107 +4059,107 @@
       </c>
       <c r="N13" s="6"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+    <row r="14" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A14" s="19">
         <v>43568</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="20">
         <v>100</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="20">
         <v>110</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="20">
         <v>392</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="20">
         <f t="shared" si="0"/>
         <v>2958</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="21">
         <f t="shared" si="1"/>
         <v>13.522650439486139</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="21">
         <f t="shared" si="2"/>
         <v>33.468559837728193</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="21">
         <f t="shared" si="3"/>
         <v>53.008789722785664</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="22">
         <v>58.9</v>
       </c>
-      <c r="J14" s="5">
+      <c r="J14" s="21">
         <f t="shared" si="4"/>
-        <v>-6.4773495605138613</v>
-      </c>
-      <c r="K14" s="5">
+        <v>-26</v>
+      </c>
+      <c r="K14" s="21">
         <f t="shared" si="5"/>
-        <v>8.4685598377281934</v>
-      </c>
-      <c r="L14" s="5">
+        <v>22</v>
+      </c>
+      <c r="L14" s="21">
         <f t="shared" si="6"/>
-        <v>-1.9912102772143356</v>
-      </c>
-      <c r="M14" s="5">
+        <v>-58</v>
+      </c>
+      <c r="M14" s="21">
         <f t="shared" si="7"/>
         <v>-142</v>
       </c>
       <c r="N14" s="6"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+    <row r="15" spans="1:14">
+      <c r="A15" s="15">
         <v>43569</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="16">
         <v>116</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="16">
         <v>97</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="16">
         <v>458</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="16">
         <f t="shared" si="0"/>
         <v>3169</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="17">
         <f t="shared" si="1"/>
         <v>14.641842852634902</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="17">
         <f t="shared" si="2"/>
         <v>27.548122436099714</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="17">
         <f t="shared" si="3"/>
         <v>57.810034711265381</v>
       </c>
-      <c r="I15" s="13">
+      <c r="I15" s="18">
         <v>59.8</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J15" s="17">
         <f t="shared" si="4"/>
-        <v>-5.3581571473650982</v>
-      </c>
-      <c r="K15" s="5">
+        <v>-10</v>
+      </c>
+      <c r="K15" s="17">
         <f t="shared" si="5"/>
-        <v>2.5481224360997139</v>
-      </c>
-      <c r="L15" s="5">
+        <v>9</v>
+      </c>
+      <c r="L15" s="17">
         <f t="shared" si="6"/>
-        <v>2.8100347112653807</v>
-      </c>
-      <c r="M15" s="5">
+        <v>8</v>
+      </c>
+      <c r="M15" s="17">
         <f t="shared" si="7"/>
         <v>69</v>
       </c>
       <c r="N15" s="6"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14">
       <c r="A16" s="4">
         <v>43570</v>
       </c>
@@ -3613,15 +4193,15 @@
       </c>
       <c r="J16" s="5">
         <f t="shared" si="4"/>
-        <v>-6.1240827218145437</v>
+        <v>-22</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" si="5"/>
-        <v>6.8212141427618391</v>
+        <v>18</v>
       </c>
       <c r="L16" s="5">
         <f t="shared" si="6"/>
-        <v>-0.69713142094730074</v>
+        <v>-43</v>
       </c>
       <c r="M16" s="5">
         <f t="shared" si="7"/>
@@ -3629,7 +4209,7 @@
       </c>
       <c r="N16" s="6"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14">
       <c r="A17" s="4">
         <v>43571</v>
       </c>
@@ -3663,15 +4243,15 @@
       </c>
       <c r="J17" s="5">
         <f t="shared" si="4"/>
-        <v>-6.0374919198448609</v>
+        <v>-18</v>
       </c>
       <c r="K17" s="5">
         <f t="shared" si="5"/>
-        <v>-4.6380090497737569</v>
+        <v>-18</v>
       </c>
       <c r="L17" s="5">
         <f t="shared" si="6"/>
-        <v>10.675500969618611</v>
+        <v>58</v>
       </c>
       <c r="M17" s="5">
         <f t="shared" si="7"/>
@@ -3679,7 +4259,7 @@
       </c>
       <c r="N17" s="6"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14">
       <c r="A18" s="4">
         <v>43572</v>
       </c>
@@ -3713,15 +4293,15 @@
       </c>
       <c r="J18" s="5">
         <f t="shared" si="4"/>
-        <v>-0.21534320323014811</v>
+        <v>21</v>
       </c>
       <c r="K18" s="5">
         <f t="shared" si="5"/>
-        <v>4.0713324360699872</v>
+        <v>8</v>
       </c>
       <c r="L18" s="5">
         <f t="shared" si="6"/>
-        <v>-3.8559892328398391</v>
+        <v>-70</v>
       </c>
       <c r="M18" s="5">
         <f t="shared" si="7"/>
@@ -3729,7 +4309,7 @@
       </c>
       <c r="N18" s="6"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14">
       <c r="A19" s="4">
         <v>43573</v>
       </c>
@@ -3763,15 +4343,15 @@
       </c>
       <c r="J19" s="5">
         <f t="shared" si="4"/>
-        <v>-3.6791147994467508</v>
+        <v>-8</v>
       </c>
       <c r="K19" s="5">
         <f t="shared" si="5"/>
-        <v>1.1410788381742769</v>
+        <v>-4</v>
       </c>
       <c r="L19" s="5">
         <f t="shared" si="6"/>
-        <v>2.5380359612724703</v>
+        <v>-34</v>
       </c>
       <c r="M19" s="5">
         <f t="shared" si="7"/>
@@ -3779,7 +4359,7 @@
       </c>
       <c r="N19" s="6"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14">
       <c r="A20" s="4">
         <v>43574</v>
       </c>
@@ -3813,15 +4393,15 @@
       </c>
       <c r="J20" s="5">
         <f t="shared" si="4"/>
-        <v>-2.4451410658307218</v>
+        <v>-14</v>
       </c>
       <c r="K20" s="5">
         <f t="shared" si="5"/>
-        <v>-2.4294670846394979</v>
+        <v>-24</v>
       </c>
       <c r="L20" s="5">
         <f t="shared" si="6"/>
-        <v>4.8746081504702232</v>
+        <v>-68</v>
       </c>
       <c r="M20" s="5">
         <f t="shared" si="7"/>
@@ -3829,107 +4409,107 @@
       </c>
       <c r="N20" s="6"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+    <row r="21" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A21" s="19">
         <v>43575</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="20">
         <v>116</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="20">
         <v>91</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="20">
         <v>410</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="20">
         <f t="shared" si="0"/>
         <v>2923</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="21">
         <f t="shared" si="1"/>
         <v>15.874101950051317</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="21">
         <f t="shared" si="2"/>
         <v>28.019158398905237</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21" s="21">
         <f t="shared" si="3"/>
         <v>56.106739651043448</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="22">
         <v>59.8</v>
       </c>
-      <c r="J21" s="5">
+      <c r="J21" s="21">
         <f t="shared" si="4"/>
-        <v>-4.1258980499486828</v>
-      </c>
-      <c r="K21" s="5">
+        <v>-10</v>
+      </c>
+      <c r="K21" s="21">
         <f t="shared" si="5"/>
-        <v>3.0191583989052369</v>
-      </c>
-      <c r="L21" s="5">
+        <v>3</v>
+      </c>
+      <c r="L21" s="21">
         <f t="shared" si="6"/>
-        <v>1.1067396510434477</v>
-      </c>
-      <c r="M21" s="5">
+        <v>-40</v>
+      </c>
+      <c r="M21" s="21">
         <f t="shared" si="7"/>
         <v>-177</v>
       </c>
       <c r="N21" s="6"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+    <row r="22" spans="1:14">
+      <c r="A22" s="15">
         <v>43576</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="16">
         <v>71</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="16">
         <v>100</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="16">
         <v>180</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="16">
         <f t="shared" si="0"/>
         <v>1904</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="17">
         <f t="shared" si="1"/>
         <v>14.915966386554622</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="17">
         <f t="shared" si="2"/>
         <v>47.268907563025209</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22" s="17">
         <f t="shared" si="3"/>
         <v>37.815126050420169</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="18">
         <v>60.4</v>
       </c>
-      <c r="J22" s="5">
+      <c r="J22" s="17">
         <f t="shared" si="4"/>
-        <v>-5.0840336134453779</v>
-      </c>
-      <c r="K22" s="5">
+        <v>-55</v>
+      </c>
+      <c r="K22" s="17">
         <f t="shared" si="5"/>
-        <v>22.268907563025209</v>
-      </c>
-      <c r="L22" s="5">
+        <v>12</v>
+      </c>
+      <c r="L22" s="17">
         <f t="shared" si="6"/>
-        <v>-17.184873949579831</v>
-      </c>
-      <c r="M22" s="5">
+        <v>-270</v>
+      </c>
+      <c r="M22" s="17">
         <f t="shared" si="7"/>
         <v>-1196</v>
       </c>
       <c r="N22" s="6"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14">
       <c r="A23" s="4">
         <v>43577</v>
       </c>
@@ -3963,15 +4543,15 @@
       </c>
       <c r="J23" s="5">
         <f t="shared" si="4"/>
-        <v>-5.0117096018735356</v>
+        <v>-14</v>
       </c>
       <c r="K23" s="5">
         <f t="shared" si="5"/>
-        <v>-1.8149882903981265</v>
+        <v>-11</v>
       </c>
       <c r="L23" s="5">
         <f t="shared" si="6"/>
-        <v>6.8266978922716675</v>
+        <v>12</v>
       </c>
       <c r="M23" s="5">
         <f t="shared" si="7"/>
@@ -3979,7 +4559,7 @@
       </c>
       <c r="N23" s="6"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14">
       <c r="A24" s="4">
         <v>43578</v>
       </c>
@@ -4013,15 +4593,15 @@
       </c>
       <c r="J24" s="5">
         <f t="shared" si="4"/>
-        <v>-2.2150363783346805</v>
+        <v>-16</v>
       </c>
       <c r="K24" s="5">
         <f t="shared" si="5"/>
-        <v>7.7405012126111572</v>
+        <v>2</v>
       </c>
       <c r="L24" s="5">
         <f t="shared" si="6"/>
-        <v>-5.5254648342764767</v>
+        <v>-144</v>
       </c>
       <c r="M24" s="5">
         <f t="shared" si="7"/>
@@ -4029,7 +4609,7 @@
       </c>
       <c r="N24" s="6"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14">
       <c r="A25" s="4">
         <v>43579</v>
       </c>
@@ -4063,15 +4643,15 @@
       </c>
       <c r="J25" s="5">
         <f t="shared" si="4"/>
-        <v>-8.2352941176470598</v>
+        <v>-50</v>
       </c>
       <c r="K25" s="5">
         <f t="shared" si="5"/>
-        <v>-1.3157894736842124</v>
+        <v>-20</v>
       </c>
       <c r="L25" s="5">
         <f t="shared" si="6"/>
-        <v>9.5510835913312775</v>
+        <v>-33</v>
       </c>
       <c r="M25" s="5">
         <f t="shared" si="7"/>
@@ -4079,7 +4659,7 @@
       </c>
       <c r="N25" s="6"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14">
       <c r="A26" s="4">
         <v>43580</v>
       </c>
@@ -4113,15 +4693,15 @@
       </c>
       <c r="J26" s="5">
         <f t="shared" si="4"/>
-        <v>-5.0085178875638832</v>
+        <v>-16</v>
       </c>
       <c r="K26" s="5">
         <f t="shared" si="5"/>
-        <v>4.1311754684838178</v>
+        <v>7</v>
       </c>
       <c r="L26" s="5">
         <f t="shared" si="6"/>
-        <v>0.87734241908006538</v>
+        <v>-40</v>
       </c>
       <c r="M26" s="5">
         <f t="shared" si="7"/>
@@ -4129,7 +4709,7 @@
       </c>
       <c r="N26" s="6"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14">
       <c r="A27" s="4">
         <v>43581</v>
       </c>
@@ -4163,15 +4743,15 @@
       </c>
       <c r="J27" s="5">
         <f t="shared" si="4"/>
-        <v>-4.7161572052401759</v>
+        <v>-56</v>
       </c>
       <c r="K27" s="5">
         <f t="shared" si="5"/>
-        <v>-1.4192139737991276</v>
+        <v>-40</v>
       </c>
       <c r="L27" s="5">
         <f t="shared" si="6"/>
-        <v>6.1353711790392964</v>
+        <v>-170</v>
       </c>
       <c r="M27" s="5">
         <f t="shared" si="7"/>
@@ -4179,132 +4759,1499 @@
       </c>
       <c r="N27" s="6"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+    <row r="28" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A28" s="19">
         <v>43582</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="20">
         <v>73</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="20">
         <v>80</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="20">
         <v>338</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="20">
         <f t="shared" si="0"/>
         <v>2364</v>
       </c>
-      <c r="F28" s="5">
+      <c r="F28" s="21">
         <f t="shared" si="1"/>
         <v>12.351945854483926</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="21">
         <f t="shared" si="2"/>
         <v>30.456852791878177</v>
       </c>
-      <c r="H28" s="5">
+      <c r="H28" s="21">
         <f t="shared" si="3"/>
         <v>57.191201353637901</v>
       </c>
-      <c r="I28" s="13">
+      <c r="I28" s="22">
         <v>60.4</v>
       </c>
-      <c r="J28" s="5">
+      <c r="J28" s="21">
         <f t="shared" si="4"/>
-        <v>-7.648054145516074</v>
-      </c>
-      <c r="K28" s="5">
+        <v>-53</v>
+      </c>
+      <c r="K28" s="21">
         <f t="shared" si="5"/>
-        <v>5.4568527918781768</v>
-      </c>
-      <c r="L28" s="5">
+        <v>-8</v>
+      </c>
+      <c r="L28" s="21">
         <f t="shared" si="6"/>
-        <v>2.1912013536379007</v>
-      </c>
-      <c r="M28" s="5">
+        <v>-112</v>
+      </c>
+      <c r="M28" s="21">
         <f t="shared" si="7"/>
         <v>-736</v>
       </c>
       <c r="N28" s="6"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+    <row r="29" spans="1:14">
+      <c r="A29" s="15">
         <v>43583</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="16">
         <v>126</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="16">
         <v>88</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="16">
         <v>407</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="16">
         <f t="shared" si="0"/>
         <v>2924</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F29" s="17">
         <f t="shared" si="1"/>
         <v>17.236662106703147</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G29" s="17">
         <f t="shared" si="2"/>
         <v>27.086183310533517</v>
       </c>
-      <c r="H29" s="5">
+      <c r="H29" s="17">
         <f t="shared" si="3"/>
         <v>55.677154582763336</v>
       </c>
-      <c r="I29" s="13">
+      <c r="I29" s="18">
         <v>60.4</v>
       </c>
-      <c r="J29" s="5">
+      <c r="J29" s="17">
         <f t="shared" si="4"/>
-        <v>-2.7633378932968533</v>
-      </c>
-      <c r="K29" s="5">
+        <v>0</v>
+      </c>
+      <c r="K29" s="17">
         <f t="shared" si="5"/>
-        <v>2.0861833105335172</v>
-      </c>
-      <c r="L29" s="5">
+        <v>0</v>
+      </c>
+      <c r="L29" s="17">
         <f t="shared" si="6"/>
-        <v>0.67715458276333607</v>
-      </c>
-      <c r="M29" s="5">
+        <v>-43</v>
+      </c>
+      <c r="M29" s="17">
         <f t="shared" si="7"/>
         <v>-176</v>
       </c>
       <c r="N29" s="6"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="7">
-        <f>AVERAGE(E11:E29)</f>
-        <v>2828.5789473684213</v>
-      </c>
-      <c r="F30" s="7">
-        <f t="shared" ref="F30:H30" si="8">AVERAGE(F11:F29)</f>
-        <v>15.370691276494002</v>
-      </c>
-      <c r="G30" s="7">
+    <row r="30" spans="1:14">
+      <c r="A30" s="4">
+        <v>43584</v>
+      </c>
+      <c r="B30" s="2">
+        <v>114</v>
+      </c>
+      <c r="C30" s="2">
+        <v>94</v>
+      </c>
+      <c r="D30" s="2">
+        <v>409</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="0"/>
+        <v>2938</v>
+      </c>
+      <c r="F30" s="5">
+        <f t="shared" si="1"/>
+        <v>15.520762423417292</v>
+      </c>
+      <c r="G30" s="5">
+        <f t="shared" si="2"/>
+        <v>28.795098706603135</v>
+      </c>
+      <c r="H30" s="5">
+        <f t="shared" si="3"/>
+        <v>55.684138869979584</v>
+      </c>
+      <c r="I30" s="13">
+        <v>60.4</v>
+      </c>
+      <c r="J30" s="5">
+        <f t="shared" si="4"/>
+        <v>-12</v>
+      </c>
+      <c r="K30" s="5">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="L30" s="5">
+        <f t="shared" si="6"/>
+        <v>-41</v>
+      </c>
+      <c r="M30" s="5">
+        <f t="shared" si="7"/>
+        <v>-162</v>
+      </c>
+      <c r="N30" s="6"/>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="4">
+        <v>43585</v>
+      </c>
+      <c r="B31" s="2">
+        <v>105</v>
+      </c>
+      <c r="C31" s="2">
+        <v>86</v>
+      </c>
+      <c r="D31" s="2">
+        <v>449</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="0"/>
+        <v>2990</v>
+      </c>
+      <c r="F31" s="5">
+        <f t="shared" si="1"/>
+        <v>14.046822742474916</v>
+      </c>
+      <c r="G31" s="5">
+        <f t="shared" si="2"/>
+        <v>25.88628762541806</v>
+      </c>
+      <c r="H31" s="5">
+        <f t="shared" si="3"/>
+        <v>60.066889632107021</v>
+      </c>
+      <c r="I31" s="13">
+        <v>60.4</v>
+      </c>
+      <c r="J31" s="5">
+        <f t="shared" si="4"/>
+        <v>-21</v>
+      </c>
+      <c r="K31" s="5">
+        <f t="shared" si="5"/>
+        <v>-2</v>
+      </c>
+      <c r="L31" s="5">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+      <c r="M31" s="5">
+        <f t="shared" si="7"/>
+        <v>-110</v>
+      </c>
+      <c r="N31" s="6"/>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="4">
+        <v>43586</v>
+      </c>
+      <c r="B32" s="2">
+        <v>146</v>
+      </c>
+      <c r="C32" s="2">
+        <v>87</v>
+      </c>
+      <c r="D32" s="2">
+        <v>385</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="0"/>
+        <v>2907</v>
+      </c>
+      <c r="F32" s="5">
+        <f t="shared" si="1"/>
+        <v>20.089439284485724</v>
+      </c>
+      <c r="G32" s="5">
+        <f t="shared" si="2"/>
+        <v>26.934984520123841</v>
+      </c>
+      <c r="H32" s="5">
+        <f t="shared" si="3"/>
+        <v>52.975576195390438</v>
+      </c>
+      <c r="I32" s="13">
+        <v>60.4</v>
+      </c>
+      <c r="J32" s="5">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="K32" s="5">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="L32" s="5">
+        <f t="shared" si="6"/>
+        <v>-65</v>
+      </c>
+      <c r="M32" s="5">
+        <f t="shared" si="7"/>
+        <v>-193</v>
+      </c>
+      <c r="N32" s="6"/>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="4">
+        <v>43587</v>
+      </c>
+      <c r="B33" s="2">
+        <v>101</v>
+      </c>
+      <c r="C33" s="2">
+        <v>50</v>
+      </c>
+      <c r="D33" s="2">
+        <v>264</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="0"/>
+        <v>1910</v>
+      </c>
+      <c r="F33" s="5">
+        <f t="shared" si="1"/>
+        <v>21.151832460732983</v>
+      </c>
+      <c r="G33" s="5">
+        <f t="shared" si="2"/>
+        <v>23.560209424083769</v>
+      </c>
+      <c r="H33" s="5">
+        <f t="shared" si="3"/>
+        <v>55.287958115183244</v>
+      </c>
+      <c r="I33" s="13">
+        <v>60.4</v>
+      </c>
+      <c r="J33" s="5">
+        <f t="shared" si="4"/>
+        <v>-25</v>
+      </c>
+      <c r="K33" s="5">
+        <f t="shared" si="5"/>
+        <v>-38</v>
+      </c>
+      <c r="L33" s="5">
+        <f t="shared" si="6"/>
+        <v>-186</v>
+      </c>
+      <c r="M33" s="5">
+        <f t="shared" si="7"/>
+        <v>-1190</v>
+      </c>
+      <c r="N33" s="6"/>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" s="4">
+        <v>43588</v>
+      </c>
+      <c r="B34" s="2">
+        <v>110</v>
+      </c>
+      <c r="C34" s="2">
+        <v>71</v>
+      </c>
+      <c r="D34" s="2">
+        <v>415</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="0"/>
+        <v>2739</v>
+      </c>
+      <c r="F34" s="5">
+        <f t="shared" si="1"/>
+        <v>16.064257028112451</v>
+      </c>
+      <c r="G34" s="5">
+        <f t="shared" si="2"/>
+        <v>23.329682365826944</v>
+      </c>
+      <c r="H34" s="5">
+        <f t="shared" si="3"/>
+        <v>60.606060606060609</v>
+      </c>
+      <c r="I34" s="13">
+        <v>60.4</v>
+      </c>
+      <c r="J34" s="5">
+        <f t="shared" si="4"/>
+        <v>-16</v>
+      </c>
+      <c r="K34" s="5">
+        <f t="shared" si="5"/>
+        <v>-17</v>
+      </c>
+      <c r="L34" s="5">
+        <f t="shared" si="6"/>
+        <v>-35</v>
+      </c>
+      <c r="M34" s="5">
+        <f t="shared" si="7"/>
+        <v>-361</v>
+      </c>
+      <c r="N34" s="6"/>
+    </row>
+    <row r="35" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A35" s="19">
+        <v>43589</v>
+      </c>
+      <c r="B35" s="20">
+        <v>65</v>
+      </c>
+      <c r="C35" s="20">
+        <v>49</v>
+      </c>
+      <c r="D35" s="20">
+        <v>327</v>
+      </c>
+      <c r="E35" s="20">
+        <f t="shared" si="0"/>
+        <v>2009</v>
+      </c>
+      <c r="F35" s="21">
+        <f t="shared" si="1"/>
+        <v>12.94176207068193</v>
+      </c>
+      <c r="G35" s="21">
+        <f t="shared" si="2"/>
+        <v>21.951219512195124</v>
+      </c>
+      <c r="H35" s="21">
+        <f t="shared" si="3"/>
+        <v>65.107018417122944</v>
+      </c>
+      <c r="I35" s="22">
+        <v>60.4</v>
+      </c>
+      <c r="J35" s="21">
+        <f t="shared" si="4"/>
+        <v>-61</v>
+      </c>
+      <c r="K35" s="21">
+        <f t="shared" si="5"/>
+        <v>-39</v>
+      </c>
+      <c r="L35" s="21">
+        <f t="shared" si="6"/>
+        <v>-123</v>
+      </c>
+      <c r="M35" s="21">
+        <f t="shared" si="7"/>
+        <v>-1091</v>
+      </c>
+      <c r="N35" s="6"/>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="15">
+        <v>43590</v>
+      </c>
+      <c r="B36" s="16">
+        <v>116</v>
+      </c>
+      <c r="C36" s="16">
+        <v>81</v>
+      </c>
+      <c r="D36" s="16">
+        <v>393</v>
+      </c>
+      <c r="E36" s="16">
+        <f t="shared" si="0"/>
+        <v>2765</v>
+      </c>
+      <c r="F36" s="17">
+        <f t="shared" si="1"/>
+        <v>16.78119349005425</v>
+      </c>
+      <c r="G36" s="17">
+        <f t="shared" si="2"/>
+        <v>26.365280289330922</v>
+      </c>
+      <c r="H36" s="17">
+        <f t="shared" si="3"/>
+        <v>56.853526220614825</v>
+      </c>
+      <c r="I36" s="18">
+        <v>60.4</v>
+      </c>
+      <c r="J36" s="17">
+        <f t="shared" si="4"/>
+        <v>-10</v>
+      </c>
+      <c r="K36" s="17">
+        <f t="shared" si="5"/>
+        <v>-7</v>
+      </c>
+      <c r="L36" s="17">
+        <f t="shared" si="6"/>
+        <v>-57</v>
+      </c>
+      <c r="M36" s="17">
+        <f t="shared" si="7"/>
+        <v>-335</v>
+      </c>
+      <c r="N36" s="6"/>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="4">
+        <v>43591</v>
+      </c>
+      <c r="B37" s="2">
+        <v>74</v>
+      </c>
+      <c r="C37" s="2">
+        <v>142</v>
+      </c>
+      <c r="D37" s="2">
+        <v>142</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" si="0"/>
+        <v>2142</v>
+      </c>
+      <c r="F37" s="5">
+        <f t="shared" si="1"/>
+        <v>13.818860877684408</v>
+      </c>
+      <c r="G37" s="5">
+        <f t="shared" si="2"/>
+        <v>59.663865546218489</v>
+      </c>
+      <c r="H37" s="5">
+        <f t="shared" si="3"/>
+        <v>26.517273576097107</v>
+      </c>
+      <c r="I37" s="13">
+        <v>60.4</v>
+      </c>
+      <c r="J37" s="5">
+        <f t="shared" si="4"/>
+        <v>-52</v>
+      </c>
+      <c r="K37" s="5">
+        <f t="shared" si="5"/>
+        <v>54</v>
+      </c>
+      <c r="L37" s="5">
+        <f t="shared" si="6"/>
+        <v>-308</v>
+      </c>
+      <c r="M37" s="5">
+        <f t="shared" si="7"/>
+        <v>-958</v>
+      </c>
+      <c r="N37" s="6"/>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="4">
+        <v>43592</v>
+      </c>
+      <c r="B38" s="2">
+        <v>65</v>
+      </c>
+      <c r="C38" s="2">
+        <v>114</v>
+      </c>
+      <c r="D38" s="2">
+        <v>276</v>
+      </c>
+      <c r="E38" s="2">
+        <f t="shared" si="0"/>
+        <v>2390</v>
+      </c>
+      <c r="F38" s="5">
+        <f t="shared" si="1"/>
+        <v>10.87866108786611</v>
+      </c>
+      <c r="G38" s="5">
+        <f t="shared" si="2"/>
+        <v>42.928870292887026</v>
+      </c>
+      <c r="H38" s="5">
+        <f t="shared" si="3"/>
+        <v>46.19246861924686</v>
+      </c>
+      <c r="I38" s="13">
+        <v>60.4</v>
+      </c>
+      <c r="J38" s="5">
+        <f t="shared" si="4"/>
+        <v>-61</v>
+      </c>
+      <c r="K38" s="5">
+        <f t="shared" si="5"/>
+        <v>26</v>
+      </c>
+      <c r="L38" s="5">
+        <f t="shared" si="6"/>
+        <v>-174</v>
+      </c>
+      <c r="M38" s="5">
+        <f t="shared" si="7"/>
+        <v>-710</v>
+      </c>
+      <c r="N38" s="6"/>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" s="4">
+        <v>43593</v>
+      </c>
+      <c r="B39" s="2">
+        <v>76</v>
+      </c>
+      <c r="C39" s="2">
+        <v>137</v>
+      </c>
+      <c r="D39" s="2">
+        <v>219</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" si="0"/>
+        <v>2413</v>
+      </c>
+      <c r="F39" s="5">
+        <f t="shared" si="1"/>
+        <v>12.598425196850393</v>
+      </c>
+      <c r="G39" s="5">
+        <f t="shared" si="2"/>
+        <v>51.098217985909656</v>
+      </c>
+      <c r="H39" s="5">
+        <f t="shared" si="3"/>
+        <v>36.303356817239951</v>
+      </c>
+      <c r="I39" s="13">
+        <v>60.4</v>
+      </c>
+      <c r="J39" s="5">
+        <f t="shared" si="4"/>
+        <v>-50</v>
+      </c>
+      <c r="K39" s="5">
+        <f t="shared" si="5"/>
+        <v>49</v>
+      </c>
+      <c r="L39" s="5">
+        <f t="shared" si="6"/>
+        <v>-231</v>
+      </c>
+      <c r="M39" s="5">
+        <f t="shared" si="7"/>
+        <v>-687</v>
+      </c>
+      <c r="N39" s="6"/>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" s="4">
+        <v>43594</v>
+      </c>
+      <c r="B40" s="2">
+        <v>80</v>
+      </c>
+      <c r="C40" s="2">
+        <v>108</v>
+      </c>
+      <c r="D40" s="2">
+        <v>205</v>
+      </c>
+      <c r="E40" s="2">
+        <f t="shared" si="0"/>
+        <v>2112</v>
+      </c>
+      <c r="F40" s="5">
+        <f t="shared" si="1"/>
+        <v>15.151515151515152</v>
+      </c>
+      <c r="G40" s="5">
+        <f t="shared" si="2"/>
+        <v>46.022727272727273</v>
+      </c>
+      <c r="H40" s="5">
+        <f t="shared" si="3"/>
+        <v>38.825757575757578</v>
+      </c>
+      <c r="I40" s="13">
+        <v>60.4</v>
+      </c>
+      <c r="J40" s="5">
+        <f t="shared" si="4"/>
+        <v>-46</v>
+      </c>
+      <c r="K40" s="5">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="L40" s="5">
+        <f t="shared" si="6"/>
+        <v>-245</v>
+      </c>
+      <c r="M40" s="5">
+        <f t="shared" si="7"/>
+        <v>-988</v>
+      </c>
+      <c r="N40" s="6"/>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" s="4">
+        <v>43595</v>
+      </c>
+      <c r="B41" s="2">
+        <v>88</v>
+      </c>
+      <c r="C41" s="2">
+        <v>56</v>
+      </c>
+      <c r="D41" s="2">
+        <v>335</v>
+      </c>
+      <c r="E41" s="2">
+        <f t="shared" si="0"/>
+        <v>2196</v>
+      </c>
+      <c r="F41" s="5">
+        <f t="shared" si="1"/>
+        <v>16.029143897996356</v>
+      </c>
+      <c r="G41" s="5">
+        <f t="shared" si="2"/>
+        <v>22.950819672131146</v>
+      </c>
+      <c r="H41" s="5">
+        <f t="shared" si="3"/>
+        <v>61.020036429872491</v>
+      </c>
+      <c r="I41" s="13">
+        <v>60.4</v>
+      </c>
+      <c r="J41" s="5">
+        <f t="shared" si="4"/>
+        <v>-38</v>
+      </c>
+      <c r="K41" s="5">
+        <f t="shared" si="5"/>
+        <v>-32</v>
+      </c>
+      <c r="L41" s="5">
+        <f t="shared" si="6"/>
+        <v>-115</v>
+      </c>
+      <c r="M41" s="5">
+        <f t="shared" si="7"/>
+        <v>-904</v>
+      </c>
+      <c r="N41" s="6"/>
+    </row>
+    <row r="42" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A42" s="19">
+        <v>43596</v>
+      </c>
+      <c r="B42" s="20">
+        <v>78</v>
+      </c>
+      <c r="C42" s="20">
+        <v>68</v>
+      </c>
+      <c r="D42" s="20">
+        <v>231</v>
+      </c>
+      <c r="E42" s="20">
+        <f t="shared" si="0"/>
+        <v>1848</v>
+      </c>
+      <c r="F42" s="21">
+        <f t="shared" si="1"/>
+        <v>16.883116883116884</v>
+      </c>
+      <c r="G42" s="21">
+        <f t="shared" si="2"/>
+        <v>33.116883116883116</v>
+      </c>
+      <c r="H42" s="21">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="I42" s="22">
+        <v>60.4</v>
+      </c>
+      <c r="J42" s="21">
+        <f t="shared" si="4"/>
+        <v>-48</v>
+      </c>
+      <c r="K42" s="21">
+        <f t="shared" si="5"/>
+        <v>-20</v>
+      </c>
+      <c r="L42" s="21">
+        <f t="shared" si="6"/>
+        <v>-219</v>
+      </c>
+      <c r="M42" s="21">
+        <f t="shared" si="7"/>
+        <v>-1252</v>
+      </c>
+      <c r="N42" s="6"/>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43" s="15">
+        <v>43597</v>
+      </c>
+      <c r="B43" s="16">
+        <v>95</v>
+      </c>
+      <c r="C43" s="16">
+        <v>103</v>
+      </c>
+      <c r="D43" s="16">
+        <v>345</v>
+      </c>
+      <c r="E43" s="16">
+        <f t="shared" si="0"/>
+        <v>2687</v>
+      </c>
+      <c r="F43" s="17">
+        <f t="shared" si="1"/>
+        <v>14.142165984369184</v>
+      </c>
+      <c r="G43" s="17">
+        <f t="shared" si="2"/>
+        <v>34.499441756605883</v>
+      </c>
+      <c r="H43" s="17">
+        <f t="shared" si="3"/>
+        <v>51.358392259024932</v>
+      </c>
+      <c r="I43" s="18">
+        <v>60.4</v>
+      </c>
+      <c r="J43" s="17">
+        <f t="shared" si="4"/>
+        <v>-31</v>
+      </c>
+      <c r="K43" s="17">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="L43" s="17">
+        <f t="shared" si="6"/>
+        <v>-105</v>
+      </c>
+      <c r="M43" s="17">
+        <f t="shared" si="7"/>
+        <v>-413</v>
+      </c>
+      <c r="N43" s="6"/>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" s="4">
+        <v>43598</v>
+      </c>
+      <c r="B44" s="2">
+        <v>77</v>
+      </c>
+      <c r="C44" s="2">
+        <v>83</v>
+      </c>
+      <c r="D44" s="2">
+        <v>284</v>
+      </c>
+      <c r="E44" s="2">
+        <f t="shared" si="0"/>
+        <v>2191</v>
+      </c>
+      <c r="F44" s="5">
+        <f t="shared" si="1"/>
+        <v>14.057507987220447</v>
+      </c>
+      <c r="G44" s="5">
+        <f t="shared" si="2"/>
+        <v>34.094020994979459</v>
+      </c>
+      <c r="H44" s="5">
+        <f t="shared" si="3"/>
+        <v>51.848471017800094</v>
+      </c>
+      <c r="I44" s="13">
+        <v>60.4</v>
+      </c>
+      <c r="J44" s="5">
+        <f t="shared" si="4"/>
+        <v>-49</v>
+      </c>
+      <c r="K44" s="5">
+        <f t="shared" si="5"/>
+        <v>-5</v>
+      </c>
+      <c r="L44" s="5">
+        <f t="shared" si="6"/>
+        <v>-166</v>
+      </c>
+      <c r="M44" s="5">
+        <f t="shared" si="7"/>
+        <v>-909</v>
+      </c>
+      <c r="N44" s="6"/>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" s="4">
+        <v>43599</v>
+      </c>
+      <c r="B45" s="2">
+        <v>130</v>
+      </c>
+      <c r="C45" s="2">
+        <v>81</v>
+      </c>
+      <c r="D45" s="2">
+        <v>523</v>
+      </c>
+      <c r="E45" s="2">
+        <f t="shared" si="0"/>
+        <v>3341</v>
+      </c>
+      <c r="F45" s="5">
+        <f t="shared" si="1"/>
+        <v>15.56420233463035</v>
+      </c>
+      <c r="G45" s="5">
+        <f t="shared" si="2"/>
+        <v>21.819814426818319</v>
+      </c>
+      <c r="H45" s="5">
+        <f t="shared" si="3"/>
+        <v>62.61598323855133</v>
+      </c>
+      <c r="I45" s="13">
+        <v>60.4</v>
+      </c>
+      <c r="J45" s="5">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="K45" s="5">
+        <f t="shared" si="5"/>
+        <v>-7</v>
+      </c>
+      <c r="L45" s="5">
+        <f t="shared" si="6"/>
+        <v>73</v>
+      </c>
+      <c r="M45" s="5">
+        <f t="shared" si="7"/>
+        <v>241</v>
+      </c>
+      <c r="N45" s="6"/>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" s="4">
+        <v>43600</v>
+      </c>
+      <c r="B46" s="2">
+        <v>69</v>
+      </c>
+      <c r="C46" s="2">
+        <v>63</v>
+      </c>
+      <c r="D46" s="2">
+        <v>348</v>
+      </c>
+      <c r="E46" s="2">
+        <f t="shared" si="0"/>
+        <v>2235</v>
+      </c>
+      <c r="F46" s="5">
+        <f t="shared" si="1"/>
+        <v>12.348993288590604</v>
+      </c>
+      <c r="G46" s="5">
+        <f t="shared" si="2"/>
+        <v>25.369127516778523</v>
+      </c>
+      <c r="H46" s="5">
+        <f t="shared" si="3"/>
+        <v>62.281879194630875</v>
+      </c>
+      <c r="I46" s="13">
+        <v>60.4</v>
+      </c>
+      <c r="J46" s="5">
+        <f t="shared" si="4"/>
+        <v>-57</v>
+      </c>
+      <c r="K46" s="5">
+        <f t="shared" si="5"/>
+        <v>-25</v>
+      </c>
+      <c r="L46" s="5">
+        <f t="shared" si="6"/>
+        <v>-102</v>
+      </c>
+      <c r="M46" s="5">
+        <f t="shared" si="7"/>
+        <v>-865</v>
+      </c>
+      <c r="N46" s="6"/>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" s="4">
+        <v>43601</v>
+      </c>
+      <c r="B47" s="2">
+        <v>101</v>
+      </c>
+      <c r="C47" s="2">
+        <v>94</v>
+      </c>
+      <c r="D47" s="2">
+        <v>411</v>
+      </c>
+      <c r="E47" s="2">
+        <f t="shared" si="0"/>
+        <v>2894</v>
+      </c>
+      <c r="F47" s="5">
+        <f t="shared" si="1"/>
+        <v>13.959917069799586</v>
+      </c>
+      <c r="G47" s="5">
+        <f t="shared" si="2"/>
+        <v>29.232895646164479</v>
+      </c>
+      <c r="H47" s="5">
+        <f t="shared" si="3"/>
+        <v>56.807187284035933</v>
+      </c>
+      <c r="I47" s="13">
+        <v>60.4</v>
+      </c>
+      <c r="J47" s="5">
+        <f t="shared" si="4"/>
+        <v>-25</v>
+      </c>
+      <c r="K47" s="5">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="L47" s="5">
+        <f t="shared" si="6"/>
+        <v>-39</v>
+      </c>
+      <c r="M47" s="5">
+        <f t="shared" si="7"/>
+        <v>-206</v>
+      </c>
+      <c r="N47" s="6"/>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" s="4">
+        <v>43602</v>
+      </c>
+      <c r="B48" s="2">
+        <v>87</v>
+      </c>
+      <c r="C48" s="2">
+        <v>63</v>
+      </c>
+      <c r="D48" s="2">
+        <v>313</v>
+      </c>
+      <c r="E48" s="2">
+        <f t="shared" si="0"/>
+        <v>2167</v>
+      </c>
+      <c r="F48" s="5">
+        <f t="shared" si="1"/>
+        <v>16.059067835717585</v>
+      </c>
+      <c r="G48" s="5">
+        <f t="shared" si="2"/>
+        <v>26.165205353022614</v>
+      </c>
+      <c r="H48" s="5">
+        <f t="shared" si="3"/>
+        <v>57.775726811259808</v>
+      </c>
+      <c r="I48" s="13">
+        <v>60.4</v>
+      </c>
+      <c r="J48" s="5">
+        <f t="shared" si="4"/>
+        <v>-39</v>
+      </c>
+      <c r="K48" s="5">
+        <f t="shared" si="5"/>
+        <v>-25</v>
+      </c>
+      <c r="L48" s="5">
+        <f t="shared" si="6"/>
+        <v>-137</v>
+      </c>
+      <c r="M48" s="5">
+        <f t="shared" si="7"/>
+        <v>-933</v>
+      </c>
+      <c r="N48" s="6"/>
+    </row>
+    <row r="49" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A49" s="19">
+        <v>43603</v>
+      </c>
+      <c r="B49" s="20">
+        <v>124</v>
+      </c>
+      <c r="C49" s="20">
+        <v>87</v>
+      </c>
+      <c r="D49" s="20">
+        <v>364</v>
+      </c>
+      <c r="E49" s="20">
+        <f t="shared" si="0"/>
+        <v>2735</v>
+      </c>
+      <c r="F49" s="21">
+        <f t="shared" si="1"/>
+        <v>18.135283363802561</v>
+      </c>
+      <c r="G49" s="21">
+        <f t="shared" si="2"/>
+        <v>28.628884826325411</v>
+      </c>
+      <c r="H49" s="21">
+        <f t="shared" si="3"/>
+        <v>53.235831809872025</v>
+      </c>
+      <c r="I49" s="22">
+        <v>61.3</v>
+      </c>
+      <c r="J49" s="21">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+      <c r="K49" s="21">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="L49" s="21">
+        <f t="shared" si="6"/>
+        <v>-86</v>
+      </c>
+      <c r="M49" s="21">
+        <f t="shared" si="7"/>
+        <v>-365</v>
+      </c>
+      <c r="N49" s="6"/>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="A50" s="15">
+        <v>43604</v>
+      </c>
+      <c r="B50" s="16">
+        <v>51</v>
+      </c>
+      <c r="C50" s="16">
+        <v>79</v>
+      </c>
+      <c r="D50" s="16">
+        <v>255</v>
+      </c>
+      <c r="E50" s="16">
+        <f t="shared" si="0"/>
+        <v>1935</v>
+      </c>
+      <c r="F50" s="17">
+        <f t="shared" si="1"/>
+        <v>10.542635658914728</v>
+      </c>
+      <c r="G50" s="17">
+        <f t="shared" si="2"/>
+        <v>36.744186046511629</v>
+      </c>
+      <c r="H50" s="17">
+        <f t="shared" si="3"/>
+        <v>52.713178294573652</v>
+      </c>
+      <c r="I50" s="18">
+        <v>61.3</v>
+      </c>
+      <c r="J50" s="17">
+        <f t="shared" si="4"/>
+        <v>-75</v>
+      </c>
+      <c r="K50" s="17">
+        <f t="shared" si="5"/>
+        <v>-9</v>
+      </c>
+      <c r="L50" s="17">
+        <f t="shared" si="6"/>
+        <v>-195</v>
+      </c>
+      <c r="M50" s="17">
+        <f t="shared" si="7"/>
+        <v>-1165</v>
+      </c>
+      <c r="N50" s="6"/>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="A51" s="4">
+        <v>43605</v>
+      </c>
+      <c r="B51" s="2">
+        <v>109</v>
+      </c>
+      <c r="C51" s="2">
+        <v>88</v>
+      </c>
+      <c r="D51" s="2">
+        <v>429</v>
+      </c>
+      <c r="E51" s="2">
+        <f t="shared" si="0"/>
+        <v>2944</v>
+      </c>
+      <c r="F51" s="5">
+        <f t="shared" si="1"/>
+        <v>14.809782608695651</v>
+      </c>
+      <c r="G51" s="5">
+        <f t="shared" si="2"/>
+        <v>26.902173913043477</v>
+      </c>
+      <c r="H51" s="5">
+        <f t="shared" si="3"/>
+        <v>58.288043478260867</v>
+      </c>
+      <c r="I51" s="13">
+        <v>61.3</v>
+      </c>
+      <c r="J51" s="5">
+        <f t="shared" si="4"/>
+        <v>-17</v>
+      </c>
+      <c r="K51" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L51" s="5">
+        <f t="shared" si="6"/>
+        <v>-21</v>
+      </c>
+      <c r="M51" s="5">
+        <f t="shared" si="7"/>
+        <v>-156</v>
+      </c>
+      <c r="N51" s="6"/>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="A52" s="4">
+        <v>43606</v>
+      </c>
+      <c r="B52" s="2">
+        <v>134</v>
+      </c>
+      <c r="C52" s="2">
+        <v>91</v>
+      </c>
+      <c r="D52" s="2">
+        <v>435</v>
+      </c>
+      <c r="E52" s="2">
+        <f t="shared" si="0"/>
+        <v>3095</v>
+      </c>
+      <c r="F52" s="5">
+        <f t="shared" si="1"/>
+        <v>17.318255250403876</v>
+      </c>
+      <c r="G52" s="5">
+        <f t="shared" si="2"/>
+        <v>26.462035541195476</v>
+      </c>
+      <c r="H52" s="5">
+        <f t="shared" si="3"/>
+        <v>56.219709208400644</v>
+      </c>
+      <c r="I52" s="13">
+        <v>61.3</v>
+      </c>
+      <c r="J52" s="5">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="K52" s="5">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L52" s="5">
+        <f t="shared" si="6"/>
+        <v>-15</v>
+      </c>
+      <c r="M52" s="5">
+        <f t="shared" si="7"/>
+        <v>-5</v>
+      </c>
+      <c r="N52" s="6"/>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="A53" s="4">
+        <v>43607</v>
+      </c>
+      <c r="B53" s="2">
+        <v>138</v>
+      </c>
+      <c r="C53" s="2">
+        <v>84</v>
+      </c>
+      <c r="D53" s="2">
+        <v>476</v>
+      </c>
+      <c r="E53" s="2">
+        <f t="shared" si="0"/>
+        <v>3212</v>
+      </c>
+      <c r="F53" s="5">
+        <f t="shared" si="1"/>
+        <v>17.185554171855539</v>
+      </c>
+      <c r="G53" s="5">
+        <f t="shared" si="2"/>
+        <v>23.536737235367372</v>
+      </c>
+      <c r="H53" s="5">
+        <f t="shared" si="3"/>
+        <v>59.277708592777088</v>
+      </c>
+      <c r="I53" s="13">
+        <v>61.3</v>
+      </c>
+      <c r="J53" s="5">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="K53" s="5">
+        <f t="shared" si="5"/>
+        <v>-4</v>
+      </c>
+      <c r="L53" s="5">
+        <f t="shared" si="6"/>
+        <v>26</v>
+      </c>
+      <c r="M53" s="5">
+        <f t="shared" si="7"/>
+        <v>112</v>
+      </c>
+      <c r="N53" s="6"/>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" s="4">
+        <v>43608</v>
+      </c>
+      <c r="B54" s="2">
+        <v>78</v>
+      </c>
+      <c r="C54" s="2">
+        <v>68</v>
+      </c>
+      <c r="D54" s="2">
+        <v>341</v>
+      </c>
+      <c r="E54" s="2">
+        <f t="shared" si="0"/>
+        <v>2288</v>
+      </c>
+      <c r="F54" s="5">
+        <f t="shared" si="1"/>
+        <v>13.636363636363635</v>
+      </c>
+      <c r="G54" s="5">
+        <f t="shared" si="2"/>
+        <v>26.74825174825175</v>
+      </c>
+      <c r="H54" s="5">
+        <f t="shared" si="3"/>
+        <v>59.615384615384613</v>
+      </c>
+      <c r="I54" s="13">
+        <v>61.3</v>
+      </c>
+      <c r="J54" s="5">
+        <f t="shared" si="4"/>
+        <v>-48</v>
+      </c>
+      <c r="K54" s="5">
+        <f t="shared" si="5"/>
+        <v>-20</v>
+      </c>
+      <c r="L54" s="5">
+        <f t="shared" si="6"/>
+        <v>-109</v>
+      </c>
+      <c r="M54" s="5">
+        <f t="shared" si="7"/>
+        <v>-812</v>
+      </c>
+      <c r="N54" s="6"/>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55" s="4">
+        <v>43609</v>
+      </c>
+      <c r="B55" s="2">
+        <v>107</v>
+      </c>
+      <c r="C55" s="2">
+        <v>93</v>
+      </c>
+      <c r="D55" s="2">
+        <v>458</v>
+      </c>
+      <c r="E55" s="2">
+        <f t="shared" si="0"/>
+        <v>3097</v>
+      </c>
+      <c r="F55" s="5">
+        <f t="shared" si="1"/>
+        <v>13.819825637713917</v>
+      </c>
+      <c r="G55" s="5">
+        <f t="shared" si="2"/>
+        <v>27.026154342912495</v>
+      </c>
+      <c r="H55" s="5">
+        <f t="shared" si="3"/>
+        <v>59.15402001937359</v>
+      </c>
+      <c r="I55" s="13">
+        <v>61.3</v>
+      </c>
+      <c r="J55" s="5">
+        <f t="shared" si="4"/>
+        <v>-19</v>
+      </c>
+      <c r="K55" s="5">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="L55" s="5">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="M55" s="5">
+        <f t="shared" si="7"/>
+        <v>-3</v>
+      </c>
+      <c r="N55" s="6"/>
+    </row>
+    <row r="56" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A56" s="19">
+        <v>43610</v>
+      </c>
+      <c r="B56" s="20">
+        <v>98</v>
+      </c>
+      <c r="C56" s="20">
+        <v>53</v>
+      </c>
+      <c r="D56" s="20">
+        <v>300</v>
+      </c>
+      <c r="E56" s="20">
+        <f t="shared" si="0"/>
+        <v>2069</v>
+      </c>
+      <c r="F56" s="21">
+        <f t="shared" si="1"/>
+        <v>18.946350894151763</v>
+      </c>
+      <c r="G56" s="21">
+        <f t="shared" si="2"/>
+        <v>23.054615756404058</v>
+      </c>
+      <c r="H56" s="21">
+        <f t="shared" si="3"/>
+        <v>57.999033349444176</v>
+      </c>
+      <c r="I56" s="22">
+        <v>61.5</v>
+      </c>
+      <c r="J56" s="21">
+        <f t="shared" si="4"/>
+        <v>-28</v>
+      </c>
+      <c r="K56" s="21">
+        <f t="shared" si="5"/>
+        <v>-35</v>
+      </c>
+      <c r="L56" s="21">
+        <f t="shared" si="6"/>
+        <v>-150</v>
+      </c>
+      <c r="M56" s="21">
+        <f t="shared" si="7"/>
+        <v>-1031</v>
+      </c>
+      <c r="N56" s="6"/>
+    </row>
+    <row r="57" spans="1:14">
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="7">
+        <f>AVERAGE(E29:E35)</f>
+        <v>2631</v>
+      </c>
+      <c r="F57" s="7">
+        <f t="shared" ref="F57:H57" si="8">AVERAGE(F50:F56)</f>
+        <v>15.179823979728445</v>
+      </c>
+      <c r="G57" s="7">
         <f t="shared" si="8"/>
-        <v>27.712801750748852</v>
-      </c>
-      <c r="H30" s="7">
+        <v>27.210593511955178</v>
+      </c>
+      <c r="H57" s="7">
         <f t="shared" si="8"/>
-        <v>56.916506972757148</v>
+        <v>57.609582508316386</v>
+      </c>
+      <c r="I57" s="7"/>
+      <c r="J57" s="7">
+        <f t="shared" ref="J57" si="9">AVERAGE(J50:J56)</f>
+        <v>-23.857142857142858</v>
+      </c>
+      <c r="K57" s="7">
+        <f t="shared" ref="K57" si="10">AVERAGE(K50:K56)</f>
+        <v>-8.5714285714285712</v>
+      </c>
+      <c r="L57" s="7">
+        <f t="shared" ref="L57" si="11">AVERAGE(L50:L56)</f>
+        <v>-65.142857142857139</v>
+      </c>
+      <c r="M57" s="7">
+        <f t="shared" ref="M57" si="12">AVERAGE(M50:M56)</f>
+        <v>-437.14285714285717</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G2:G29" formula="1"/>
+    <ignoredError sqref="G2:G29 G30:G35 G36:G42 G43:G49 G50:G56" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>